<commit_message>
work hard play hard
</commit_message>
<xml_diff>
--- a/.idea/issues_maturities.xlsx
+++ b/.idea/issues_maturities.xlsx
@@ -709,10 +709,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>20072700</t>
-        </is>
+      <c r="A20" t="n">
+        <v>20072700</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>

</xml_diff>